<commit_message>
WIP BiblioPhilly descriptive MD mapping
</commit_message>
<xml_diff>
--- a/doc/BiblioPhillyFieldCheckList.xlsx
+++ b/doc/BiblioPhillyFieldCheckList.xlsx
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="115">
   <si>
     <t>Administrative information (not for publication)</t>
   </si>
@@ -729,6 +729,12 @@
   </si>
   <si>
     <t>history/origin/origDate/@notAfter</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>first value is contributor, subsequent are cataloguers</t>
   </si>
 </sst>
 </file>
@@ -739,7 +745,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -796,20 +802,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -819,10 +879,24 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E72" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E72"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="TEI" dataDxfId="4"/>
+    <tableColumn id="2" name="Column" dataDxfId="3"/>
+    <tableColumn id="3" name="In metadata.xml?" dataDxfId="2"/>
+    <tableColumn id="4" name="in tei?" dataDxfId="1"/>
+    <tableColumn id="5" name="Note" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Crop">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Crop">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -830,109 +904,49 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="191B0E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EFEDE3"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="8C8D86"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E6C069"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="897B61"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8DAB8E"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="77A2BB"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="E28394"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="77A2BB"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="957A99"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Crop">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Franklin Gothic Book" panose="020B0503020102020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Franklin Gothic Book" panose="020B0503020102020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Crop">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -941,23 +955,23 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="67000"/>
+                <a:satMod val="105000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:tint val="73000"/>
+                <a:satMod val="103000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="81000"/>
+                <a:satMod val="109000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -967,23 +981,23 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
                 <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:shade val="100000"/>
                 <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:shade val="78000"/>
+                <a:satMod val="120000"/>
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -991,26 +1005,23 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="in">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="34925" cap="flat" cmpd="sng" algn="in">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="in">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1024,7 +1035,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1045,16 +1056,16 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:shade val="98000"/>
                 <a:satMod val="150000"/>
-                <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:shade val="90000"/>
                 <a:satMod val="130000"/>
-                <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
@@ -1074,7 +1085,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Crop" id="{EC9488ED-E761-4D60-9AC4-764D1FE2C171}" vid="{CE19780C-D67D-4C13-9DE9-A52BC3BA51B4}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1082,720 +1093,891 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="C14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="C15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="C16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="C17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="C22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="C23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="C24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="C25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="C27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="C29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="C30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="C31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="C32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="C33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="C34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="C36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="C37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="C38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="C39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="C40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="C41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="C42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="C43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="C44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="C45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="C46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="C47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="C48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="C49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="C51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="C52" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C53" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="C53" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="C55" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+      <c r="C56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="C58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="C59" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
+      <c r="B60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="C61" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="4"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="C62" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="5"/>
+      <c r="B63" s="6"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+      <c r="C64" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="C65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5"/>
+      <c r="B66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+      <c r="C67" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="4"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="7" t="s">
+      <c r="C68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
+      <c r="B70" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add BiblioPhilly elements to browse page
Simplify language text in b-phil TEI

Correct FLP name

Fix tests
</commit_message>
<xml_diff>
--- a/doc/BiblioPhillyFieldCheckList.xlsx
+++ b/doc/BiblioPhillyFieldCheckList.xlsx
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="118">
   <si>
     <t>Administrative information (not for publication)</t>
   </si>
@@ -735,6 +735,15 @@
   </si>
   <si>
     <t>first value is contributor, subsequent are cataloguers</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>HTML: Date text in origin details</t>
+  </si>
+  <si>
+    <t>Translated to text</t>
   </si>
 </sst>
 </file>
@@ -832,7 +841,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
@@ -880,14 +892,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E72" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E72"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="TEI" dataDxfId="4"/>
-    <tableColumn id="2" name="Column" dataDxfId="3"/>
-    <tableColumn id="3" name="In metadata.xml?" dataDxfId="2"/>
-    <tableColumn id="4" name="in tei?" dataDxfId="1"/>
-    <tableColumn id="5" name="Note" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F72" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F72"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="TEI" dataDxfId="5"/>
+    <tableColumn id="2" name="Column" dataDxfId="4"/>
+    <tableColumn id="3" name="In metadata.xml?" dataDxfId="3"/>
+    <tableColumn id="4" name="in tei?" dataDxfId="2"/>
+    <tableColumn id="6" name="HTML" dataDxfId="0"/>
+    <tableColumn id="5" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1093,11 +1106,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,12 +1118,12 @@
     <col min="1" max="1" width="54.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="4" max="5" width="7.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -1123,17 +1136,20 @@
       <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1147,7 +1163,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1161,17 +1177,17 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1184,11 +1200,11 @@
       <c r="D7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1202,7 +1218,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1215,8 +1231,11 @@
       <c r="D9" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1229,8 +1248,11 @@
       <c r="D10" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1243,8 +1265,11 @@
       <c r="D11" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1257,8 +1282,11 @@
       <c r="D12" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1271,8 +1299,11 @@
       <c r="D13" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1285,8 +1316,11 @@
       <c r="D14" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1299,8 +1333,11 @@
       <c r="D15" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1313,8 +1350,11 @@
       <c r="D16" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1327,8 +1367,11 @@
       <c r="D17" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -1341,8 +1384,11 @@
       <c r="D18" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
@@ -1355,8 +1401,11 @@
       <c r="D19" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
@@ -1369,8 +1418,11 @@
       <c r="D20" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1383,8 +1435,11 @@
       <c r="D21" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>34</v>
       </c>
@@ -1397,8 +1452,11 @@
       <c r="D22" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
@@ -1411,8 +1469,11 @@
       <c r="D23" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -1425,8 +1486,11 @@
       <c r="D24" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -1439,8 +1503,11 @@
       <c r="D25" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1453,8 +1520,11 @@
       <c r="D26" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
@@ -1467,12 +1537,15 @@
       <c r="D27" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
@@ -1485,8 +1558,14 @@
       <c r="D29" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>111</v>
       </c>
@@ -1499,8 +1578,14 @@
       <c r="D30" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>112</v>
       </c>
@@ -1513,8 +1598,14 @@
       <c r="D31" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
@@ -1527,8 +1618,14 @@
       <c r="D32" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>52</v>
       </c>
@@ -1541,8 +1638,11 @@
       <c r="D33" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
@@ -1555,12 +1655,15 @@
       <c r="D34" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>56</v>
       </c>
@@ -1573,8 +1676,11 @@
       <c r="D36" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
@@ -1587,8 +1693,14 @@
       <c r="D37" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>60</v>
       </c>
@@ -1601,8 +1713,11 @@
       <c r="D38" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>62</v>
       </c>
@@ -1615,8 +1730,11 @@
       <c r="D39" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>64</v>
       </c>
@@ -1629,8 +1747,11 @@
       <c r="D40" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
@@ -1643,8 +1764,11 @@
       <c r="D41" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
@@ -1657,8 +1781,11 @@
       <c r="D42" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>70</v>
       </c>
@@ -1671,8 +1798,11 @@
       <c r="D43" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>72</v>
       </c>
@@ -1685,8 +1815,11 @@
       <c r="D44" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>74</v>
       </c>
@@ -1699,8 +1832,11 @@
       <c r="D45" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>76</v>
       </c>
@@ -1713,8 +1849,11 @@
       <c r="D46" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>78</v>
       </c>
@@ -1727,8 +1866,11 @@
       <c r="D47" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>80</v>
       </c>
@@ -1741,8 +1883,11 @@
       <c r="D48" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>82</v>
       </c>
@@ -1755,12 +1900,15 @@
       <c r="D49" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>84</v>
       </c>
@@ -1773,8 +1921,11 @@
       <c r="D51" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>62</v>
       </c>
@@ -1787,8 +1938,11 @@
       <c r="D52" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>62</v>
       </c>
@@ -1801,12 +1955,15 @@
       <c r="D53" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>88</v>
       </c>
@@ -1819,8 +1976,11 @@
       <c r="D55" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>90</v>
       </c>
@@ -1833,12 +1993,15 @@
       <c r="D56" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>92</v>
       </c>
@@ -1851,8 +2014,11 @@
       <c r="D58" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>94</v>
       </c>
@@ -1865,12 +2031,15 @@
       <c r="D59" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>92</v>
       </c>
@@ -1883,8 +2052,11 @@
       <c r="D61" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>94</v>
       </c>
@@ -1897,12 +2069,15 @@
       <c r="D62" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>92</v>
       </c>
@@ -1915,8 +2090,11 @@
       <c r="D64" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>94</v>
       </c>
@@ -1929,12 +2107,15 @@
       <c r="D65" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>100</v>
       </c>
@@ -1947,8 +2128,11 @@
       <c r="D67" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>102</v>
       </c>
@@ -1961,12 +2145,15 @@
       <c r="D68" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
       <c r="B70" s="6" t="s">
         <v>104</v>
@@ -1975,6 +2162,9 @@
         <v>110</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>